<commit_message>
Add large file using Git LFS
</commit_message>
<xml_diff>
--- a/performance_eval.xlsx
+++ b/performance_eval.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kun\Desktop\slide-classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF96C0F-7A3F-4FE1-BBC8-5FCDEDD24402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3027A039-83BC-44E7-8030-ADC06C4B41F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="8445" windowWidth="19440" windowHeight="15000" tabRatio="536" xr2:uid="{56D6BA94-91E7-564B-8B5F-E8479AFD178B}"/>
+    <workbookView xWindow="-19320" yWindow="8445" windowWidth="19440" windowHeight="15000" tabRatio="536" activeTab="1" xr2:uid="{56D6BA94-91E7-564B-8B5F-E8479AFD178B}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Adv_visual" sheetId="3" r:id="rId4"/>
     <sheet name="Adv_multimodal" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="90">
   <si>
     <t>advance</t>
   </si>
@@ -253,9 +253,6 @@
     <t>*</t>
   </si>
   <si>
-    <t>textual and visual fusion model</t>
-  </si>
-  <si>
     <t>Baseline</t>
   </si>
   <si>
@@ -276,6 +273,33 @@
   <si>
     <t>Choose the best
 configuration in each type</t>
+  </si>
+  <si>
+    <t>N gram</t>
+  </si>
+  <si>
+    <t>K Best features</t>
+  </si>
+  <si>
+    <t>NB_t (unigram, bigram)</t>
+  </si>
+  <si>
+    <t>unigram, bigram</t>
+  </si>
+  <si>
+    <t>NB_tv(unigram, bigram)</t>
+  </si>
+  <si>
+    <t>NB_t F1-score</t>
+  </si>
+  <si>
+    <t>NB_v F1-score</t>
+  </si>
+  <si>
+    <t>NB_tv F1-score</t>
+  </si>
+  <si>
+    <t>improvement(+/-)</t>
   </si>
 </sst>
 </file>
@@ -339,7 +363,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -352,8 +376,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -426,11 +468,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="mediumDashed">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -549,25 +600,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -579,28 +640,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1051,8 +1105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B2877B-CC65-9149-BC13-59F5E87F1C8A}">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9"/>
@@ -1132,7 +1186,7 @@
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="48" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="5">
@@ -1161,7 +1215,7 @@
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="44"/>
+      <c r="A10" s="49"/>
       <c r="B10" s="2">
         <v>16</v>
       </c>
@@ -1188,7 +1242,7 @@
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="47"/>
+      <c r="A11" s="50"/>
       <c r="B11" s="6">
         <v>16</v>
       </c>
@@ -1215,7 +1269,7 @@
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="48" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="2">
@@ -1244,7 +1298,7 @@
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="44"/>
+      <c r="A13" s="49"/>
       <c r="B13" s="2">
         <v>16</v>
       </c>
@@ -1271,7 +1325,7 @@
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="47"/>
+      <c r="A14" s="50"/>
       <c r="B14" s="2">
         <v>16</v>
       </c>
@@ -1298,7 +1352,7 @@
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="48" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="5">
@@ -1330,7 +1384,7 @@
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="44"/>
+      <c r="A16" s="49"/>
       <c r="B16" s="2">
         <v>16</v>
       </c>
@@ -1357,7 +1411,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="16.3" thickBot="1">
-      <c r="A17" s="48"/>
+      <c r="A17" s="51"/>
       <c r="B17" s="3">
         <v>16</v>
       </c>
@@ -1384,7 +1438,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="16.3" thickTop="1">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="52" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="2">
@@ -1413,7 +1467,7 @@
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="44"/>
+      <c r="A19" s="49"/>
       <c r="B19" s="2">
         <v>4</v>
       </c>
@@ -1440,7 +1494,7 @@
       </c>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="47"/>
+      <c r="A20" s="50"/>
       <c r="B20" s="2">
         <v>4</v>
       </c>
@@ -1467,7 +1521,7 @@
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="48" t="s">
         <v>11</v>
       </c>
       <c r="B21" s="5">
@@ -1499,7 +1553,7 @@
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="44"/>
+      <c r="A22" s="49"/>
       <c r="B22" s="2">
         <v>4</v>
       </c>
@@ -1526,7 +1580,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="16.3" thickBot="1">
-      <c r="A23" s="48"/>
+      <c r="A23" s="51"/>
       <c r="B23" s="3">
         <v>4</v>
       </c>
@@ -1553,7 +1607,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="16.3" thickTop="1">
-      <c r="A24" s="46" t="s">
+      <c r="A24" s="52" t="s">
         <v>13</v>
       </c>
       <c r="B24" s="4">
@@ -1582,7 +1636,7 @@
       </c>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="44"/>
+      <c r="A25" s="49"/>
       <c r="B25" s="2">
         <v>8</v>
       </c>
@@ -1609,7 +1663,7 @@
       </c>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="47"/>
+      <c r="A26" s="50"/>
       <c r="B26" s="2">
         <v>8</v>
       </c>
@@ -1636,7 +1690,7 @@
       </c>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="49" t="s">
+      <c r="A27" s="53" t="s">
         <v>14</v>
       </c>
       <c r="B27" s="5">
@@ -1665,7 +1719,7 @@
       </c>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="50"/>
+      <c r="A28" s="54"/>
       <c r="B28" s="2">
         <v>8</v>
       </c>
@@ -1692,7 +1746,7 @@
       </c>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="51"/>
+      <c r="A29" s="55"/>
       <c r="B29" s="6">
         <v>8</v>
       </c>
@@ -1722,7 +1776,7 @@
       </c>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="43" t="s">
+      <c r="A30" s="48" t="s">
         <v>15</v>
       </c>
       <c r="B30" s="2">
@@ -1751,7 +1805,7 @@
       </c>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="44"/>
+      <c r="A31" s="49"/>
       <c r="B31" s="2">
         <v>8</v>
       </c>
@@ -1778,7 +1832,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="16.3" thickBot="1">
-      <c r="A32" s="45"/>
+      <c r="A32" s="58"/>
       <c r="B32" s="10">
         <v>8</v>
       </c>
@@ -1807,21 +1861,21 @@
     </row>
     <row r="33" spans="1:9" ht="16.3" thickTop="1"/>
     <row r="35" spans="1:9" ht="32.15" thickBot="1">
-      <c r="A35" s="52" t="s">
-        <v>81</v>
+      <c r="A35" s="42" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="16.3" thickTop="1">
-      <c r="A36" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="B36" s="42" t="s">
+      <c r="A36" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="56"/>
       <c r="G36" s="41"/>
       <c r="H36" s="11"/>
       <c r="I36" s="11"/>
@@ -1845,13 +1899,13 @@
       <c r="F37" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G37" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="H37" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="I37" s="55" t="s">
+      <c r="G37" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I37" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1860,28 +1914,28 @@
         <v>22</v>
       </c>
       <c r="B38" s="1">
-        <v>0.80359999999999998</v>
+        <v>0.82120000000000004</v>
       </c>
       <c r="C38" s="1">
-        <v>0.63890000000000002</v>
+        <v>0.67</v>
       </c>
       <c r="D38" s="1">
-        <v>0.64949999999999997</v>
+        <v>0.68600000000000005</v>
       </c>
       <c r="E38" s="1">
-        <v>0.76919999999999999</v>
+        <v>0.79049999999999998</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G38" s="55" t="s">
-        <v>77</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H38" s="1">
+        <v>5500</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1901,61 +1955,61 @@
         <v>0.5968</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G39" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="16.3" thickBot="1">
+      <c r="A40" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0.91659999999999997</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0.68340000000000001</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0.7198</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H39" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B40" s="1">
-        <v>0.81789999999999996</v>
-      </c>
-      <c r="C40" s="1">
-        <v>0.63319999999999999</v>
-      </c>
-      <c r="D40" s="1">
-        <v>0.65500000000000003</v>
-      </c>
-      <c r="E40" s="1">
-        <v>0.77190000000000003</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G40" s="57" t="s">
-        <v>77</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>77</v>
+      <c r="G40" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H40" s="1">
+        <v>2500</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B41" s="54" t="s">
+      <c r="A41" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="54"/>
-      <c r="D41" s="54"/>
-      <c r="E41" s="54"/>
-      <c r="F41" s="54"/>
-      <c r="G41" s="53"/>
-      <c r="H41" s="53"/>
-      <c r="I41" s="53"/>
+      <c r="C41" s="57"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="57"/>
+      <c r="F41" s="57"/>
+      <c r="G41" s="47"/>
+      <c r="H41" s="47"/>
+      <c r="I41" s="47"/>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="2" t="s">
@@ -1976,13 +2030,13 @@
       <c r="F42" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G42" s="55" t="s">
+      <c r="G42" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H42" s="55" t="s">
+      <c r="H42" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I42" s="55" t="s">
+      <c r="I42" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2005,7 +2059,7 @@
       <c r="F43" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G43" s="55">
+      <c r="G43" s="1">
         <v>16</v>
       </c>
       <c r="H43" s="38">
@@ -2034,7 +2088,7 @@
       <c r="F44" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G44" s="55">
+      <c r="G44" s="1">
         <v>4</v>
       </c>
       <c r="H44" s="38">
@@ -2076,6 +2130,8 @@
     <row r="46" spans="1:9" ht="16.3" thickTop="1"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B41:F41"/>
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="A21:A23"/>
@@ -2084,8 +2140,6 @@
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="A27:A29"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B41:F41"/>
   </mergeCells>
   <conditionalFormatting sqref="E9:E17">
     <cfRule type="expression" dxfId="14" priority="16">
@@ -2170,24 +2224,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4588EAFA-B8B1-4CFC-82C3-85B35A9999FB}">
-  <dimension ref="A1:S18"/>
+  <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.9"/>
   <cols>
     <col min="1" max="1" width="27.35546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.2109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.2109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.92578125" customWidth="1"/>
+    <col min="7" max="7" width="8.78515625" customWidth="1"/>
     <col min="8" max="8" width="27.35546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="27.35546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B1" s="58" t="s">
+      <c r="A1" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="43" t="s">
         <v>30</v>
       </c>
       <c r="C1" t="s">
@@ -2199,10 +2258,10 @@
       <c r="E1" t="s">
         <v>33</v>
       </c>
-      <c r="H1" t="s">
-        <v>79</v>
-      </c>
-      <c r="I1" s="58" t="s">
+      <c r="H1" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" s="43" t="s">
         <v>30</v>
       </c>
       <c r="J1" t="s">
@@ -2214,10 +2273,10 @@
       <c r="L1" t="s">
         <v>33</v>
       </c>
-      <c r="O1" t="s">
-        <v>78</v>
-      </c>
-      <c r="P1" s="58" t="s">
+      <c r="O1" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="P1" s="43" t="s">
         <v>30</v>
       </c>
       <c r="Q1" t="s">
@@ -2231,26 +2290,26 @@
       </c>
     </row>
     <row r="2" spans="1:19">
-      <c r="A2" s="59"/>
-      <c r="O2" s="59"/>
+      <c r="A2" s="44"/>
+      <c r="O2" s="44"/>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="43" t="s">
         <v>34</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.78949999999999998</v>
+        <v>0.84209999999999996</v>
       </c>
       <c r="D3">
-        <v>0.88239999999999996</v>
+        <v>0.9143</v>
       </c>
       <c r="E3">
         <v>19</v>
       </c>
-      <c r="H3" s="58" t="s">
+      <c r="H3" s="43" t="s">
         <v>34</v>
       </c>
       <c r="I3">
@@ -2265,7 +2324,7 @@
       <c r="L3">
         <v>19</v>
       </c>
-      <c r="O3" s="58" t="s">
+      <c r="O3" s="43" t="s">
         <v>34</v>
       </c>
       <c r="P3">
@@ -2282,22 +2341,22 @@
       </c>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="43" t="s">
         <v>36</v>
       </c>
       <c r="B4">
-        <v>0.90239999999999998</v>
+        <v>0.88100000000000001</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>0.94869999999999999</v>
+        <v>0.93669999999999998</v>
       </c>
       <c r="E4">
         <v>37</v>
       </c>
-      <c r="H4" s="58" t="s">
+      <c r="H4" s="43" t="s">
         <v>36</v>
       </c>
       <c r="I4">
@@ -2312,7 +2371,7 @@
       <c r="L4">
         <v>37</v>
       </c>
-      <c r="O4" s="58" t="s">
+      <c r="O4" s="43" t="s">
         <v>36</v>
       </c>
       <c r="P4">
@@ -2329,22 +2388,22 @@
       </c>
     </row>
     <row r="5" spans="1:19">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="43" t="s">
         <v>37</v>
       </c>
       <c r="B5">
-        <v>0.63639999999999997</v>
+        <v>0.76</v>
       </c>
       <c r="C5">
-        <v>0.53849999999999998</v>
+        <v>0.73080000000000001</v>
       </c>
       <c r="D5">
-        <v>0.58330000000000004</v>
+        <v>0.74509999999999998</v>
       </c>
       <c r="E5">
         <v>26</v>
       </c>
-      <c r="H5" s="58" t="s">
+      <c r="H5" s="43" t="s">
         <v>37</v>
       </c>
       <c r="I5">
@@ -2359,39 +2418,39 @@
       <c r="L5">
         <v>26</v>
       </c>
-      <c r="O5" s="58" t="s">
+      <c r="O5" s="43" t="s">
         <v>37</v>
       </c>
       <c r="P5">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="Q5">
+        <v>0.61539999999999995</v>
+      </c>
+      <c r="R5">
         <v>0.66669999999999996</v>
-      </c>
-      <c r="Q5">
-        <v>0.46150000000000002</v>
-      </c>
-      <c r="R5">
-        <v>0.54549999999999998</v>
       </c>
       <c r="S5">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="43" t="s">
         <v>38</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
-        <v>0.1111</v>
+        <v>0.22220000000000001</v>
       </c>
       <c r="D6">
-        <v>0.2</v>
+        <v>0.36359999999999998</v>
       </c>
       <c r="E6">
         <v>9</v>
       </c>
-      <c r="H6" s="58" t="s">
+      <c r="H6" s="43" t="s">
         <v>38</v>
       </c>
       <c r="I6">
@@ -2406,24 +2465,24 @@
       <c r="L6">
         <v>9</v>
       </c>
-      <c r="O6" s="58" t="s">
+      <c r="O6" s="43" t="s">
         <v>38</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>0.22220000000000001</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>0.36359999999999998</v>
       </c>
       <c r="S6">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="43" t="s">
         <v>39</v>
       </c>
       <c r="B7">
@@ -2438,7 +2497,7 @@
       <c r="E7">
         <v>37</v>
       </c>
-      <c r="H7" s="58" t="s">
+      <c r="H7" s="43" t="s">
         <v>39</v>
       </c>
       <c r="I7">
@@ -2453,39 +2512,39 @@
       <c r="L7">
         <v>37</v>
       </c>
-      <c r="O7" s="58" t="s">
+      <c r="O7" s="43" t="s">
         <v>39</v>
       </c>
       <c r="P7">
         <v>1</v>
       </c>
       <c r="Q7">
-        <v>0.94589999999999996</v>
+        <v>0.97299999999999998</v>
       </c>
       <c r="R7">
-        <v>0.97219999999999995</v>
+        <v>0.98629999999999995</v>
       </c>
       <c r="S7">
         <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:19">
-      <c r="A8" s="58" t="s">
+      <c r="A8" s="43" t="s">
         <v>40</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8">
-        <v>0.9</v>
+        <v>0.93330000000000002</v>
       </c>
       <c r="D8">
-        <v>0.94740000000000002</v>
+        <v>0.96550000000000002</v>
       </c>
       <c r="E8">
         <v>30</v>
       </c>
-      <c r="H8" s="58" t="s">
+      <c r="H8" s="43" t="s">
         <v>40</v>
       </c>
       <c r="I8">
@@ -2500,7 +2559,7 @@
       <c r="L8">
         <v>30</v>
       </c>
-      <c r="O8" s="58" t="s">
+      <c r="O8" s="43" t="s">
         <v>40</v>
       </c>
       <c r="P8">
@@ -2517,22 +2576,22 @@
       </c>
     </row>
     <row r="9" spans="1:19">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="43" t="s">
         <v>41</v>
       </c>
       <c r="B9">
-        <v>0.90239999999999998</v>
+        <v>0.94589999999999996</v>
       </c>
       <c r="C9">
-        <v>0.90239999999999998</v>
+        <v>0.85370000000000001</v>
       </c>
       <c r="D9">
-        <v>0.90239999999999998</v>
+        <v>0.89739999999999998</v>
       </c>
       <c r="E9">
         <v>41</v>
       </c>
-      <c r="H9" s="58" t="s">
+      <c r="H9" s="43" t="s">
         <v>41</v>
       </c>
       <c r="I9">
@@ -2547,39 +2606,39 @@
       <c r="L9">
         <v>41</v>
       </c>
-      <c r="O9" s="58" t="s">
+      <c r="O9" s="43" t="s">
         <v>41</v>
       </c>
       <c r="P9">
-        <v>0.92859999999999998</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="Q9">
         <v>0.95120000000000005</v>
       </c>
       <c r="R9">
-        <v>0.93979999999999997</v>
+        <v>0.96299999999999997</v>
       </c>
       <c r="S9">
         <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="43" t="s">
         <v>42</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10">
-        <v>0.61899999999999999</v>
+        <v>0.57140000000000002</v>
       </c>
       <c r="D10">
-        <v>0.76470000000000005</v>
+        <v>0.72729999999999995</v>
       </c>
       <c r="E10">
         <v>21</v>
       </c>
-      <c r="H10" s="58" t="s">
+      <c r="H10" s="43" t="s">
         <v>42</v>
       </c>
       <c r="I10">
@@ -2594,24 +2653,24 @@
       <c r="L10">
         <v>21</v>
       </c>
-      <c r="O10" s="58" t="s">
+      <c r="O10" s="43" t="s">
         <v>42</v>
       </c>
       <c r="P10">
         <v>1</v>
       </c>
       <c r="Q10">
-        <v>0.52380000000000004</v>
+        <v>0.57140000000000002</v>
       </c>
       <c r="R10">
-        <v>0.6875</v>
+        <v>0.72729999999999995</v>
       </c>
       <c r="S10">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="58" t="s">
+      <c r="A11" s="43" t="s">
         <v>43</v>
       </c>
       <c r="B11">
@@ -2626,7 +2685,7 @@
       <c r="E11">
         <v>10</v>
       </c>
-      <c r="H11" s="58" t="s">
+      <c r="H11" s="43" t="s">
         <v>43</v>
       </c>
       <c r="I11">
@@ -2641,7 +2700,7 @@
       <c r="L11">
         <v>10</v>
       </c>
-      <c r="O11" s="58" t="s">
+      <c r="O11" s="43" t="s">
         <v>43</v>
       </c>
       <c r="P11">
@@ -2658,22 +2717,22 @@
       </c>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="58" t="s">
+      <c r="A12" s="43" t="s">
         <v>44</v>
       </c>
       <c r="B12">
-        <v>0.54649999999999999</v>
+        <v>0.52629999999999999</v>
       </c>
       <c r="C12">
-        <v>0.83930000000000005</v>
+        <v>0.89290000000000003</v>
       </c>
       <c r="D12">
-        <v>0.66200000000000003</v>
+        <v>0.6623</v>
       </c>
       <c r="E12">
         <v>56</v>
       </c>
-      <c r="H12" s="58" t="s">
+      <c r="H12" s="43" t="s">
         <v>44</v>
       </c>
       <c r="I12">
@@ -2688,39 +2747,39 @@
       <c r="L12">
         <v>56</v>
       </c>
-      <c r="O12" s="58" t="s">
+      <c r="O12" s="43" t="s">
         <v>44</v>
       </c>
       <c r="P12">
-        <v>0.68059999999999998</v>
+        <v>0.69330000000000003</v>
       </c>
       <c r="Q12">
-        <v>0.875</v>
+        <v>0.92859999999999998</v>
       </c>
       <c r="R12">
-        <v>0.76559999999999995</v>
+        <v>0.79390000000000005</v>
       </c>
       <c r="S12">
         <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="58" t="s">
+      <c r="A13" s="43" t="s">
         <v>45</v>
       </c>
       <c r="B13">
-        <v>0.65590000000000004</v>
+        <v>0.74070000000000003</v>
       </c>
       <c r="C13">
-        <v>0.91039999999999999</v>
+        <v>0.89549999999999996</v>
       </c>
       <c r="D13">
-        <v>0.76249999999999996</v>
+        <v>0.81079999999999997</v>
       </c>
       <c r="E13">
         <v>67</v>
       </c>
-      <c r="H13" s="58" t="s">
+      <c r="H13" s="43" t="s">
         <v>45</v>
       </c>
       <c r="I13">
@@ -2735,39 +2794,39 @@
       <c r="L13">
         <v>67</v>
       </c>
-      <c r="O13" s="58" t="s">
+      <c r="O13" s="43" t="s">
         <v>45</v>
       </c>
       <c r="P13">
-        <v>0.53849999999999998</v>
+        <v>0.6038</v>
       </c>
       <c r="Q13">
-        <v>0.94030000000000002</v>
+        <v>0.95520000000000005</v>
       </c>
       <c r="R13">
-        <v>0.68479999999999996</v>
+        <v>0.7399</v>
       </c>
       <c r="S13">
         <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="43" t="s">
         <v>46</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14">
-        <v>8.3299999999999999E-2</v>
+        <v>0.125</v>
       </c>
       <c r="D14">
-        <v>0.15379999999999999</v>
+        <v>0.22220000000000001</v>
       </c>
       <c r="E14">
         <v>24</v>
       </c>
-      <c r="H14" s="58" t="s">
+      <c r="H14" s="43" t="s">
         <v>46</v>
       </c>
       <c r="I14">
@@ -2782,38 +2841,38 @@
       <c r="L14">
         <v>24</v>
       </c>
-      <c r="O14" s="58" t="s">
+      <c r="O14" s="43" t="s">
         <v>46</v>
       </c>
       <c r="P14">
         <v>1</v>
       </c>
       <c r="Q14">
-        <v>8.3299999999999999E-2</v>
+        <v>0.16669999999999999</v>
       </c>
       <c r="R14">
-        <v>0.15379999999999999</v>
+        <v>0.28570000000000001</v>
       </c>
       <c r="S14">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="O15" s="59"/>
+      <c r="A15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="O15" s="44"/>
     </row>
     <row r="16" spans="1:19">
-      <c r="A16" s="58" t="s">
+      <c r="A16" s="43" t="s">
         <v>35</v>
       </c>
       <c r="D16">
-        <v>0.76919999999999999</v>
+        <v>0.79049999999999998</v>
       </c>
       <c r="E16">
         <v>377</v>
       </c>
-      <c r="H16" s="58" t="s">
+      <c r="H16" s="43" t="s">
         <v>35</v>
       </c>
       <c r="K16">
@@ -2822,33 +2881,33 @@
       <c r="L16">
         <v>377</v>
       </c>
-      <c r="O16" s="58" t="s">
+      <c r="O16" s="43" t="s">
         <v>35</v>
       </c>
       <c r="R16">
-        <v>0.77190000000000003</v>
+        <v>0.80900000000000005</v>
       </c>
       <c r="S16">
         <v>377</v>
       </c>
     </row>
     <row r="17" spans="1:19">
-      <c r="A17" s="58" t="s">
+      <c r="A17" s="43" t="s">
         <v>47</v>
       </c>
       <c r="B17">
-        <v>0.80359999999999998</v>
+        <v>0.82120000000000004</v>
       </c>
       <c r="C17">
-        <v>0.63890000000000002</v>
+        <v>0.67</v>
       </c>
       <c r="D17">
-        <v>0.64949999999999997</v>
+        <v>0.68600000000000005</v>
       </c>
       <c r="E17">
         <v>377</v>
       </c>
-      <c r="H17" s="58" t="s">
+      <c r="H17" s="43" t="s">
         <v>47</v>
       </c>
       <c r="I17">
@@ -2863,39 +2922,39 @@
       <c r="L17">
         <v>377</v>
       </c>
-      <c r="O17" s="58" t="s">
+      <c r="O17" s="43" t="s">
         <v>47</v>
       </c>
       <c r="P17">
-        <v>0.81789999999999996</v>
+        <v>0.91659999999999997</v>
       </c>
       <c r="Q17">
-        <v>0.63319999999999999</v>
+        <v>0.68340000000000001</v>
       </c>
       <c r="R17">
-        <v>0.65500000000000003</v>
+        <v>0.7198</v>
       </c>
       <c r="S17">
         <v>377</v>
       </c>
     </row>
     <row r="18" spans="1:19">
-      <c r="A18" s="58" t="s">
+      <c r="A18" s="43" t="s">
         <v>48</v>
       </c>
       <c r="B18">
-        <v>0.79969999999999997</v>
+        <v>0.82289999999999996</v>
       </c>
       <c r="C18">
-        <v>0.76919999999999999</v>
+        <v>0.79049999999999998</v>
       </c>
       <c r="D18">
-        <v>0.73909999999999998</v>
+        <v>0.76639999999999997</v>
       </c>
       <c r="E18">
         <v>377</v>
       </c>
-      <c r="H18" s="58" t="s">
+      <c r="H18" s="43" t="s">
         <v>48</v>
       </c>
       <c r="I18">
@@ -2910,24 +2969,255 @@
       <c r="L18">
         <v>377</v>
       </c>
-      <c r="O18" s="58" t="s">
+      <c r="O18" s="43" t="s">
         <v>48</v>
       </c>
       <c r="P18">
-        <v>0.81589999999999996</v>
+        <v>0.86250000000000004</v>
       </c>
       <c r="Q18">
-        <v>0.77190000000000003</v>
+        <v>0.80900000000000005</v>
       </c>
       <c r="R18">
-        <v>0.74350000000000005</v>
+        <v>0.78910000000000002</v>
       </c>
       <c r="S18">
         <v>377</v>
       </c>
     </row>
+    <row r="24" spans="1:19">
+      <c r="B24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" t="s">
+        <v>88</v>
+      </c>
+      <c r="E24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
+      <c r="A25" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="60">
+        <v>0.9143</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0.8125</v>
+      </c>
+      <c r="E25" s="61">
+        <f>D25-B25</f>
+        <v>-0.1018</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="A26" s="59" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="60">
+        <v>0.93669999999999998</v>
+      </c>
+      <c r="C26">
+        <v>0.78790000000000004</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <f t="shared" ref="E26:E36" si="0">D26-B26</f>
+        <v>6.3300000000000023E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
+      <c r="A27" s="59" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="60">
+        <v>0.74509999999999998</v>
+      </c>
+      <c r="C27">
+        <v>0.59089999999999998</v>
+      </c>
+      <c r="D27">
+        <v>0.66669999999999996</v>
+      </c>
+      <c r="E27" s="61">
+        <f t="shared" si="0"/>
+        <v>-7.8400000000000025E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
+      <c r="A28" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="60">
+        <v>0.36359999999999998</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0.36359999999999998</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
+      <c r="A29" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="60">
+        <v>0.98629999999999995</v>
+      </c>
+      <c r="C29">
+        <v>0.82669999999999999</v>
+      </c>
+      <c r="D29">
+        <v>0.98629999999999995</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
+      <c r="A30" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="60">
+        <v>0.96550000000000002</v>
+      </c>
+      <c r="C30">
+        <v>0.9153</v>
+      </c>
+      <c r="D30">
+        <v>0.96550000000000002</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
+      <c r="A31" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="60">
+        <v>0.89739999999999998</v>
+      </c>
+      <c r="C31">
+        <v>0.82930000000000004</v>
+      </c>
+      <c r="D31">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>6.5599999999999992E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
+      <c r="A32" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="60">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0.72729999999999995</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="E33" s="62">
+        <f t="shared" si="0"/>
+        <v>0.33329999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="59" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="60">
+        <v>0.6623</v>
+      </c>
+      <c r="C34">
+        <v>0.61760000000000004</v>
+      </c>
+      <c r="D34">
+        <v>0.79390000000000005</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>0.13160000000000005</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="60">
+        <v>0.81079999999999997</v>
+      </c>
+      <c r="C35">
+        <v>0.49759999999999999</v>
+      </c>
+      <c r="D35">
+        <v>0.7399</v>
+      </c>
+      <c r="E35" s="61">
+        <f t="shared" si="0"/>
+        <v>-7.0899999999999963E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="59" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="60">
+        <v>0.22220000000000001</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0.28570000000000001</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>6.3500000000000001E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2935,8 +3225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9585E41-EF43-4E30-A762-64D5175E5819}">
   <dimension ref="A1:S59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.9"/>
@@ -5206,7 +5496,7 @@
   <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.9"/>
@@ -6756,7 +7046,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE4A792A-D05A-4A6C-82A1-66A369AF65E8}">
   <dimension ref="A1:S60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="R38" sqref="R38"/>
     </sheetView>
   </sheetViews>
@@ -9018,12 +9308,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6dec70a8-b87c-41aa-8c24-c4316beda457" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9268,17 +9557,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6dec70a8-b87c-41aa-8c24-c4316beda457" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24F1D1CE-7581-4207-BB38-A627B144EEA7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8DEEE3D-8557-45CA-A391-79A8792ECB69}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6dec70a8-b87c-41aa-8c24-c4316beda457"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7a14eb4d-97ee-4433-895e-cd1987fea1f2"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9303,18 +9602,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8DEEE3D-8557-45CA-A391-79A8792ECB69}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24F1D1CE-7581-4207-BB38-A627B144EEA7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6dec70a8-b87c-41aa-8c24-c4316beda457"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7a14eb4d-97ee-4433-895e-cd1987fea1f2"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>